<commit_message>
add name for compartment
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/2_species_1_reaction.xlsx
+++ b/tests/multialgorithm/fixtures/2_species_1_reaction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22540" windowHeight="14260" tabRatio="989" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22540" windowHeight="14260" tabRatio="989" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="78">
   <si>
     <t>Id</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>cytosol</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1231,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCellId="1" sqref="C3 A1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1266,7 +1269,6 @@
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1292,11 +1294,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCellId="1" sqref="C3 A1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1325,7 +1327,9 @@
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1579,7 +1583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
update the example model and the code so a) the model changes mass during the simulation, and b) the code includes a line that obtains the mass of a compartment at a particular time
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/2_species_1_reaction.xlsx
+++ b/tests/multialgorithm/fixtures/2_species_1_reaction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22540" windowHeight="14260" tabRatio="989" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37900" windowHeight="21140" tabRatio="989" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -221,9 +221,6 @@
     <t>forward</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Coefficient</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t>cytosol</t>
+  </si>
+  <si>
+    <t>"100"</t>
   </si>
 </sst>
 </file>
@@ -345,12 +345,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -776,14 +779,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCellId="1" sqref="C3 A1"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -815,8 +821,8 @@
       <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>52</v>
+      <c r="C2" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -854,10 +860,10 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -934,7 +940,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>32</v>
@@ -951,7 +957,7 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -962,14 +968,14 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -985,7 +991,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -996,7 +1002,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1069,46 +1075,46 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>11</v>
@@ -1136,10 +1142,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
@@ -1148,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>39</v>
@@ -1157,13 +1163,13 @@
         <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1328,7 +1334,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -1354,7 +1360,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCellId="1" sqref="C3 A1"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1402,7 +1408,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
@@ -1422,7 +1428,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">

</xml_diff>